<commit_message>
Wrote some results, added S1 File.
</commit_message>
<xml_diff>
--- a/archive/tables.xlsx
+++ b/archive/tables.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Biology</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Note. All times given are medians.</t>
   </si>
   <si>
-    <t>Estimate</t>
-  </si>
-  <si>
     <t>Intercept</t>
   </si>
   <si>
@@ -84,12 +81,21 @@
   </si>
   <si>
     <t>Conflict of interest</t>
+  </si>
+  <si>
+    <t>Estimate (review)</t>
+  </si>
+  <si>
+    <t>Estimate (production)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,12 +140,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,166 +655,225 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A1:B19"/>
+      <selection sqref="A1:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="5">
+        <v>4.1873790849999999</v>
+      </c>
+      <c r="C2" s="5">
+        <v>4.2495693188519699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B2">
-        <v>4.1873790849999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="5">
+        <v>1.885353E-3</v>
+      </c>
+      <c r="C3" s="5">
+        <v>5.9158296383032896E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B3">
-        <v>1.885353E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="5">
+        <v>-7.2180000000000002E-6</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-1.4879271769975999E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
-        <v>-7.2180000000000002E-6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" s="5">
+        <v>-9.3400899999999997E-4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4.3176025642281702E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B5">
-        <v>-9.3400899999999997E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" s="5">
+        <v>-1.0995199999999999E-4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>-1.11718223359496E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B6">
-        <v>-1.0995199999999999E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>-1.899822E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="5">
+        <v>4.9118132407661597E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2004</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>0.68772862099999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="5">
+        <v>0.101646745352951</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2005</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>0.73865381699999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="5">
+        <v>-0.12942827953389399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2006</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>0.69365071099999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="5">
+        <v>-0.109288525365644</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2007</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>0.54891641599999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="5">
+        <v>-0.46095013149497499</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2008</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>0.61999715600000005</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="5">
+        <v>-0.57019108715497102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2009</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <v>0.59294335099999995</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="5">
+        <v>-0.56629724829058503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2010</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="5">
         <v>0.65820246999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="5">
+        <v>-0.66378718583387797</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <v>0.65243934999999997</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="5">
+        <v>-0.56771495041387299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2012</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <v>0.73469631199999996</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="5">
+        <v>-0.47268199440374897</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2013</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="5">
         <v>0.73683272899999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="5">
+        <v>-0.37085600483803999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2014</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <v>0.77307768399999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="5">
+        <v>-0.53778005058935596</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2015</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="5">
         <v>0.84419351200000003</v>
+      </c>
+      <c r="C19" s="5">
+        <v>-0.24988634171385199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>